<commit_message>
update: cleaning unused from this modular code
</commit_message>
<xml_diff>
--- a/api/logs/log_configllm.xlsx
+++ b/api/logs/log_configllm.xlsx
@@ -466,7 +466,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-11-22 19:49:52</t>
+          <t>2024-11-25 19:15:26</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -496,7 +496,7 @@
         <v>200</v>
       </c>
       <c r="H2" t="n">
-        <v>1000</v>
+        <v>1082</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: create new vectordb
</commit_message>
<xml_diff>
--- a/api/logs/log_configllm.xlsx
+++ b/api/logs/log_configllm.xlsx
@@ -466,7 +466,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-11-25 19:15:26</t>
+          <t>2024-12-11 12:44:01</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -496,7 +496,7 @@
         <v>200</v>
       </c>
       <c r="H2" t="n">
-        <v>1082</v>
+        <v>1121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>